<commit_message>
script for metanalysis added
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">instr</t>
   </si>
@@ -21,6 +21,18 @@
   </si>
   <si>
     <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_n_control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_n_active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg_active_age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg_control_age</t>
   </si>
   <si>
     <t xml:space="preserve">avg_baseline_mean_act</t>
@@ -541,25 +553,41 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="F2" s="1" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H2" s="1" t="e">
         <v>#NUM!</v>
       </c>
@@ -576,25 +604,37 @@
         <v>#NUM!</v>
       </c>
       <c r="O2" s="1"/>
+      <c r="P2" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F3" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H3" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -611,25 +651,37 @@
         <v>#NUM!</v>
       </c>
       <c r="O3" s="2"/>
+      <c r="P3" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F4" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H4" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -646,166 +698,214 @@
         <v>#NUM!</v>
       </c>
       <c r="O4" s="2"/>
+      <c r="P4" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="n">
+        <v>209</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>210</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>14.97</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>14.97</v>
+      </c>
+      <c r="H5" s="2" t="n">
         <v>43.5</v>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="n">
+      <c r="I5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
         <v>44.2</v>
       </c>
-      <c r="G5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="n">
+      <c r="K5" s="2" t="n">
+        <v>0.282842712474618</v>
+      </c>
+      <c r="L5" s="2" t="n">
         <v>27.8</v>
       </c>
-      <c r="I5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2" t="n">
+      <c r="M5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="n">
         <v>38.95</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="O5" s="2" t="n">
         <v>2.33345237791561</v>
       </c>
-      <c r="L5" s="2" t="n">
+      <c r="P5" s="2" t="n">
         <v>-1.15018315018315</v>
       </c>
-      <c r="M5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2" t="n">
+      <c r="Q5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="n">
         <v>-0.392255962574663</v>
       </c>
-      <c r="O5" s="2" t="n">
+      <c r="S5" s="2" t="n">
         <v>0.176208139031742</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D6" s="2" t="n">
+        <v>161</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>253</v>
+      </c>
+      <c r="F6" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G6" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H6" s="2" t="n">
         <v>21.6066666666667</v>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>3.90129892898934</v>
-      </c>
-      <c r="F6" s="2" t="n">
+      <c r="I6" s="2" t="n">
+        <v>1.895793589327</v>
+      </c>
+      <c r="J6" s="2" t="n">
         <v>18.99</v>
       </c>
-      <c r="G6" s="2" t="n">
-        <v>5.20406571826298</v>
-      </c>
-      <c r="H6" s="2" t="n">
+      <c r="K6" s="2" t="n">
+        <v>1.16988603433554</v>
+      </c>
+      <c r="L6" s="2" t="n">
         <v>10.9733333333333</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="M6" s="2" t="n">
         <v>2.9759256263108</v>
       </c>
-      <c r="J6" s="2" t="n">
+      <c r="N6" s="2" t="n">
         <v>13.7466666666667</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="O6" s="2" t="n">
         <v>4.91468547654205</v>
       </c>
-      <c r="L6" s="2" t="n">
+      <c r="P6" s="2" t="n">
         <v>-1.12611988022129</v>
       </c>
-      <c r="M6" s="2" t="n">
+      <c r="Q6" s="2" t="n">
         <v>0.286097061706614</v>
       </c>
-      <c r="N6" s="2" t="n">
+      <c r="R6" s="2" t="n">
         <v>-0.506105006105006</v>
       </c>
-      <c r="O6" s="2" t="n">
+      <c r="S6" s="2" t="n">
         <v>0.0562697385464052</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D7" s="2" t="n">
+        <v>658</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>679</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>15.8975</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>15.8975</v>
+      </c>
+      <c r="H7" s="2" t="n">
         <v>23.6705</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>6.52625747108918</v>
-      </c>
-      <c r="F7" s="2" t="n">
+      <c r="I7" s="2" t="n">
+        <v>2.65185257985114</v>
+      </c>
+      <c r="J7" s="2" t="n">
         <v>22.9795</v>
       </c>
-      <c r="G7" s="2" t="n">
-        <v>6.85459237146509</v>
-      </c>
-      <c r="H7" s="2" t="n">
+      <c r="K7" s="2" t="n">
+        <v>2.75376278457027</v>
+      </c>
+      <c r="L7" s="2" t="n">
         <v>11.7575</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="M7" s="2" t="n">
         <v>5.00914518918306</v>
       </c>
-      <c r="J7" s="2" t="n">
+      <c r="N7" s="2" t="n">
         <v>17.8565</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="O7" s="2" t="n">
         <v>6.6560920057849</v>
       </c>
-      <c r="L7" s="2" t="n">
+      <c r="P7" s="2" t="n">
         <v>-1.63100033703923</v>
       </c>
-      <c r="M7" s="2" t="n">
+      <c r="Q7" s="2" t="n">
         <v>1.31802595898147</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="R7" s="2" t="n">
         <v>-0.601378145829666</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="S7" s="2" t="n">
         <v>0.625188776821564</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E8" s="2"/>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F8" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H8" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -822,72 +922,96 @@
         <v>#NUM!</v>
       </c>
       <c r="O8" s="2"/>
+      <c r="P8" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>13.54</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>13.54</v>
+      </c>
+      <c r="H9" s="2" t="n">
         <v>48.556</v>
       </c>
-      <c r="E9" s="2" t="n">
-        <v>3.70774594598929</v>
-      </c>
-      <c r="F9" s="2" t="n">
+      <c r="I9" s="2" t="n">
+        <v>2.0571290674141</v>
+      </c>
+      <c r="J9" s="2" t="n">
         <v>41.374</v>
       </c>
-      <c r="G9" s="2" t="n">
-        <v>3.84551426989941</v>
-      </c>
-      <c r="H9" s="2" t="n">
+      <c r="K9" s="2" t="n">
+        <v>3.21606902910992</v>
+      </c>
+      <c r="L9" s="2" t="n">
         <v>16.178</v>
       </c>
-      <c r="I9" s="2" t="n">
+      <c r="M9" s="2" t="n">
         <v>0.808498608533125</v>
       </c>
-      <c r="J9" s="2" t="n">
+      <c r="N9" s="2" t="n">
         <v>30.078</v>
       </c>
-      <c r="K9" s="2" t="n">
+      <c r="O9" s="2" t="n">
         <v>13.4953147425319</v>
       </c>
-      <c r="L9" s="2" t="n">
+      <c r="P9" s="2" t="n">
         <v>-2.06506081209349</v>
       </c>
-      <c r="M9" s="2" t="n">
+      <c r="Q9" s="2" t="n">
         <v>0.218537778971517</v>
       </c>
-      <c r="N9" s="2" t="n">
+      <c r="R9" s="2" t="n">
         <v>-0.659844596408108</v>
       </c>
-      <c r="O9" s="2" t="n">
+      <c r="S9" s="2" t="n">
         <v>1.06191966398227</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E10" s="2"/>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F10" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H10" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -904,72 +1028,96 @@
         <v>#NUM!</v>
       </c>
       <c r="O10" s="2"/>
+      <c r="P10" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D11" s="2" t="n">
+        <v>216</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>226</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>14.7822222222222</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>14.7822222222222</v>
+      </c>
+      <c r="H11" s="2" t="n">
         <v>32.1544444444444</v>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>29.3985739922497</v>
-      </c>
-      <c r="F11" s="2" t="n">
+      <c r="I11" s="2" t="n">
+        <v>2.20080730137324</v>
+      </c>
+      <c r="J11" s="2" t="n">
         <v>30.0533333333333</v>
       </c>
-      <c r="G11" s="2" t="n">
-        <v>27.3780605595064</v>
-      </c>
-      <c r="H11" s="2" t="n">
+      <c r="K11" s="2" t="n">
+        <v>2.83738337988444</v>
+      </c>
+      <c r="L11" s="2" t="n">
         <v>27.6433333333333</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="M11" s="2" t="n">
         <v>28.1645703855038</v>
       </c>
-      <c r="J11" s="2" t="n">
+      <c r="N11" s="2" t="n">
         <v>28.2955555555556</v>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="O11" s="2" t="n">
         <v>29.9785648885629</v>
       </c>
-      <c r="L11" s="2" t="n">
+      <c r="P11" s="2" t="n">
         <v>-0.766537651364512</v>
       </c>
-      <c r="M11" s="2" t="n">
+      <c r="Q11" s="2" t="n">
         <v>0.738100761848697</v>
       </c>
-      <c r="N11" s="2" t="n">
+      <c r="R11" s="2" t="n">
         <v>-0.413957059870753</v>
       </c>
-      <c r="O11" s="2" t="n">
+      <c r="S11" s="2" t="n">
         <v>0.595212113379861</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E12" s="2"/>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F12" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H12" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -986,166 +1134,214 @@
         <v>#NUM!</v>
       </c>
       <c r="O12" s="2"/>
+      <c r="P12" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>23</v>
       </c>
       <c r="D13" s="2" t="n">
+        <v>804</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>826</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>12.5977272727273</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>12.5977272727273</v>
+      </c>
+      <c r="H13" s="2" t="n">
         <v>21.7127272727273</v>
       </c>
-      <c r="E13" s="2" t="n">
-        <v>5.83141997068114</v>
-      </c>
-      <c r="F13" s="2" t="n">
+      <c r="I13" s="2" t="n">
+        <v>1.84699562997395</v>
+      </c>
+      <c r="J13" s="2" t="n">
         <v>20.3345454545455</v>
       </c>
-      <c r="G13" s="2" t="n">
-        <v>6.28488112345259</v>
-      </c>
-      <c r="H13" s="2" t="n">
+      <c r="K13" s="2" t="n">
+        <v>2.58903484498981</v>
+      </c>
+      <c r="L13" s="2" t="n">
         <v>12.0717391304348</v>
       </c>
-      <c r="I13" s="2" t="n">
+      <c r="M13" s="2" t="n">
         <v>3.85507888396347</v>
       </c>
-      <c r="J13" s="2" t="n">
+      <c r="N13" s="2" t="n">
         <v>16.9395652173913</v>
       </c>
-      <c r="K13" s="2" t="n">
+      <c r="O13" s="2" t="n">
         <v>5.6824670364687</v>
       </c>
-      <c r="L13" s="2" t="n">
+      <c r="P13" s="2" t="n">
         <v>-1.15683202443842</v>
       </c>
-      <c r="M13" s="2" t="n">
+      <c r="Q13" s="2" t="n">
         <v>0.616974044793137</v>
       </c>
-      <c r="N13" s="2" t="n">
+      <c r="R13" s="2" t="n">
         <v>-0.380298979613213</v>
       </c>
-      <c r="O13" s="2" t="n">
+      <c r="S13" s="2" t="n">
         <v>0.680937833475856</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>26</v>
       </c>
       <c r="D14" s="2" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>2128</v>
+      </c>
+      <c r="F14" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G14" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H14" s="2" t="n">
         <v>57.5021052631579</v>
       </c>
-      <c r="E14" s="2" t="n">
-        <v>3.52352030243015</v>
-      </c>
-      <c r="F14" s="2" t="n">
+      <c r="I14" s="2" t="n">
+        <v>2.60477491944167</v>
+      </c>
+      <c r="J14" s="2" t="n">
         <v>57.4957894736842</v>
       </c>
-      <c r="G14" s="2" t="n">
-        <v>3.54585566509141</v>
-      </c>
-      <c r="H14" s="2" t="n">
+      <c r="K14" s="2" t="n">
+        <v>2.72964623558229</v>
+      </c>
+      <c r="L14" s="2" t="n">
         <v>35.1913333333333</v>
       </c>
-      <c r="I14" s="2" t="n">
+      <c r="M14" s="2" t="n">
         <v>1.3935917964878</v>
       </c>
-      <c r="J14" s="2" t="n">
+      <c r="N14" s="2" t="n">
         <v>37.412</v>
       </c>
-      <c r="K14" s="2" t="n">
+      <c r="O14" s="2" t="n">
         <v>3.87342631639888</v>
       </c>
-      <c r="L14" s="2" t="n">
+      <c r="P14" s="2" t="n">
         <v>-2.2756000958178</v>
       </c>
-      <c r="M14" s="2" t="n">
+      <c r="Q14" s="2" t="n">
         <v>0.826862337778918</v>
       </c>
-      <c r="N14" s="2" t="n">
+      <c r="R14" s="2" t="n">
         <v>-1.96011632040328</v>
       </c>
-      <c r="O14" s="2" t="n">
+      <c r="S14" s="2" t="n">
         <v>0.875318084876132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>8</v>
       </c>
       <c r="D15" s="2" t="n">
+        <v>215</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>201</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>13.80375</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>13.80375</v>
+      </c>
+      <c r="H15" s="2" t="n">
         <v>47.8928571428571</v>
       </c>
-      <c r="E15" s="2" t="n">
-        <v>12.253269923148</v>
-      </c>
-      <c r="F15" s="2" t="n">
+      <c r="I15" s="2" t="n">
+        <v>4.1924643281556</v>
+      </c>
+      <c r="J15" s="2" t="n">
         <v>45.1657142857143</v>
       </c>
-      <c r="G15" s="2" t="n">
-        <v>14.2387614830584</v>
-      </c>
-      <c r="H15" s="2" t="n">
+      <c r="K15" s="2" t="n">
+        <v>3.54110959204275</v>
+      </c>
+      <c r="L15" s="2" t="n">
         <v>32.4457142857143</v>
       </c>
-      <c r="I15" s="2" t="n">
+      <c r="M15" s="2" t="n">
         <v>7.47242454437839</v>
       </c>
-      <c r="J15" s="2" t="n">
+      <c r="N15" s="2" t="n">
         <v>35.0257142857143</v>
       </c>
-      <c r="K15" s="2" t="n">
+      <c r="O15" s="2" t="n">
         <v>6.61467776273054</v>
       </c>
-      <c r="L15" s="2" t="n">
+      <c r="P15" s="2" t="n">
         <v>-1.98483574563368</v>
       </c>
-      <c r="M15" s="2" t="n">
+      <c r="Q15" s="2" t="n">
         <v>1.38937759873451</v>
       </c>
-      <c r="N15" s="2" t="n">
+      <c r="R15" s="2" t="n">
         <v>-1.39269623963861</v>
       </c>
-      <c r="O15" s="2" t="n">
+      <c r="S15" s="2" t="n">
         <v>1.30755814489424</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E16" s="2"/>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F16" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H16" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1162,72 +1358,96 @@
         <v>#NUM!</v>
       </c>
       <c r="O16" s="2"/>
+      <c r="P16" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D17" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>11.17</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>11.17</v>
+      </c>
+      <c r="H17" s="2" t="n">
         <v>71.75</v>
       </c>
-      <c r="E17" s="2" t="n">
-        <v>0.91923881554252</v>
-      </c>
-      <c r="F17" s="2" t="n">
+      <c r="I17" s="2" t="n">
+        <v>0.0494974746830585</v>
+      </c>
+      <c r="J17" s="2" t="n">
         <v>67.56</v>
       </c>
-      <c r="G17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2" t="n">
+      <c r="K17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="n">
         <v>52.62</v>
       </c>
-      <c r="I17" s="2" t="n">
+      <c r="M17" s="2" t="n">
         <v>3.50724963468528</v>
       </c>
-      <c r="J17" s="2" t="n">
+      <c r="N17" s="2" t="n">
         <v>61.09</v>
       </c>
-      <c r="K17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2" t="n">
+      <c r="O17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2" t="n">
         <v>-1.88141575073107</v>
       </c>
-      <c r="M17" s="2" t="n">
+      <c r="Q17" s="2" t="n">
         <v>0.654746986929079</v>
       </c>
-      <c r="N17" s="2" t="n">
+      <c r="R17" s="2" t="n">
         <v>-0.374746597161888</v>
       </c>
-      <c r="O17" s="2" t="n">
+      <c r="S17" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D18" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E18" s="2"/>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F18" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H18" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1244,72 +1464,96 @@
         <v>#NUM!</v>
       </c>
       <c r="O18" s="2"/>
+      <c r="P18" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>13</v>
       </c>
       <c r="D19" s="2" t="n">
+        <v>509</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>541</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>15.4653846153846</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>15.4653846153846</v>
+      </c>
+      <c r="H19" s="2" t="n">
         <v>22.1481818181818</v>
       </c>
-      <c r="E19" s="2" t="n">
-        <v>7.39583101237693</v>
-      </c>
-      <c r="F19" s="2" t="n">
+      <c r="I19" s="2" t="n">
+        <v>2.13475993966535</v>
+      </c>
+      <c r="J19" s="2" t="n">
         <v>22.3363636363636</v>
       </c>
-      <c r="G19" s="2" t="n">
-        <v>7.11567744171596</v>
-      </c>
-      <c r="H19" s="2" t="n">
+      <c r="K19" s="2" t="n">
+        <v>3.46703174068382</v>
+      </c>
+      <c r="L19" s="2" t="n">
         <v>14.6654545454545</v>
       </c>
-      <c r="I19" s="2" t="n">
+      <c r="M19" s="2" t="n">
         <v>7.5560483900467</v>
       </c>
-      <c r="J19" s="2" t="n">
+      <c r="N19" s="2" t="n">
         <v>19.6636363636364</v>
       </c>
-      <c r="K19" s="2" t="n">
+      <c r="O19" s="2" t="n">
         <v>6.29988773348744</v>
       </c>
-      <c r="L19" s="2" t="n">
+      <c r="P19" s="2" t="n">
         <v>-1.02786088724732</v>
       </c>
-      <c r="M19" s="2" t="n">
+      <c r="Q19" s="2" t="n">
         <v>0.717959167358529</v>
       </c>
-      <c r="N19" s="2" t="n">
+      <c r="R19" s="2" t="n">
         <v>-0.315175193070365</v>
       </c>
-      <c r="O19" s="2" t="n">
+      <c r="S19" s="2" t="n">
         <v>0.323783853617054</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="D20" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E20" s="2"/>
+      <c r="D20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F20" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H20" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1326,25 +1570,37 @@
         <v>#NUM!</v>
       </c>
       <c r="O20" s="2"/>
+      <c r="P20" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D21" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E21" s="2"/>
+      <c r="D21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F21" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H21" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1361,25 +1617,37 @@
         <v>#NUM!</v>
       </c>
       <c r="O21" s="2"/>
+      <c r="P21" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D22" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E22" s="2"/>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F22" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H22" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1396,60 +1664,84 @@
         <v>#NUM!</v>
       </c>
       <c r="O22" s="2"/>
+      <c r="P22" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="H23" s="2" t="n">
         <v>24.2</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="n">
-        <v>21.6</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2" t="n">
-        <v>17.2</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="n">
-        <v>23.93</v>
+        <v>21.6</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2" t="n">
-        <v>-0.78125</v>
+        <v>17.2</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2" t="n">
+        <v>23.93</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2" t="n">
+        <v>-0.78125</v>
+      </c>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2" t="n">
         <v>0.20610349402919</v>
       </c>
-      <c r="O23" s="2"/>
+      <c r="S23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D24" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E24" s="2"/>
+      <c r="D24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F24" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H24" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1466,95 +1758,131 @@
         <v>#NUM!</v>
       </c>
       <c r="O24" s="2"/>
+      <c r="P24" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>11.77</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>11.77</v>
+      </c>
+      <c r="H25" s="2" t="n">
         <v>10.44</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2" t="n">
-        <v>11.33</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2" t="n">
-        <v>5.13</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2" t="n">
-        <v>6.65</v>
+        <v>11.33</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2" t="n">
-        <v>-1.18791946308725</v>
+        <v>5.13</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2" t="n">
+        <v>-1.18791946308725</v>
+      </c>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2" t="n">
         <v>-1.00970873786408</v>
       </c>
-      <c r="O25" s="2"/>
+      <c r="S25" s="2"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F26" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G26" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H26" s="2" t="n">
         <v>37.6</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="n">
-        <v>38.6</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2" t="n">
-        <v>54.2</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2" t="n">
-        <v>48.9</v>
+        <v>38.6</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2" t="n">
-        <v>1.77540106951872</v>
+        <v>54.2</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2" t="n">
+        <v>48.9</v>
+      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2" t="n">
+        <v>1.77540106951872</v>
+      </c>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2" t="n">
         <v>1.02487562189055</v>
       </c>
-      <c r="O26" s="2"/>
+      <c r="S26" s="2"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D27" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E27" s="2"/>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F27" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H27" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1571,252 +1899,324 @@
         <v>#NUM!</v>
       </c>
       <c r="O27" s="2"/>
+      <c r="P27" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S27" s="2"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D28" s="2" t="n">
+        <v>438</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>457</v>
+      </c>
+      <c r="F28" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G28" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H28" s="2" t="n">
         <v>19.1414285714286</v>
       </c>
-      <c r="E28" s="2" t="n">
-        <v>3.71034332899903</v>
-      </c>
-      <c r="F28" s="2" t="n">
+      <c r="I28" s="2" t="n">
+        <v>0.68668284770579</v>
+      </c>
+      <c r="J28" s="2" t="n">
         <v>19.73</v>
       </c>
-      <c r="G28" s="2" t="n">
-        <v>3.68908751138634</v>
-      </c>
-      <c r="H28" s="2" t="n">
+      <c r="K28" s="2" t="n">
+        <v>0.681682093200692</v>
+      </c>
+      <c r="L28" s="2" t="n">
         <v>10.1716666666667</v>
       </c>
-      <c r="I28" s="2" t="n">
+      <c r="M28" s="2" t="n">
         <v>2.09659167857422</v>
       </c>
-      <c r="J28" s="2" t="n">
+      <c r="N28" s="2" t="n">
         <v>11.6683333333333</v>
       </c>
-      <c r="K28" s="2" t="n">
+      <c r="O28" s="2" t="n">
         <v>2.42543535610963</v>
       </c>
-      <c r="L28" s="2" t="n">
+      <c r="P28" s="2" t="n">
         <v>-1.81433607742254</v>
       </c>
-      <c r="M28" s="2" t="n">
+      <c r="Q28" s="2" t="n">
         <v>1.05185624392889</v>
       </c>
-      <c r="N28" s="2" t="n">
+      <c r="R28" s="2" t="n">
         <v>-1.49139968116527</v>
       </c>
-      <c r="O28" s="2" t="n">
+      <c r="S28" s="2" t="n">
         <v>0.262979127241591</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>11</v>
       </c>
       <c r="D29" s="2" t="n">
+        <v>356</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>352</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>15.6909090909091</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>15.6909090909091</v>
+      </c>
+      <c r="H29" s="2" t="n">
         <v>13.2318181818182</v>
       </c>
-      <c r="E29" s="2" t="n">
-        <v>6.48560994538188</v>
-      </c>
-      <c r="F29" s="2" t="n">
+      <c r="I29" s="2" t="n">
+        <v>1.77901913730828</v>
+      </c>
+      <c r="J29" s="2" t="n">
         <v>12.4327272727273</v>
       </c>
-      <c r="G29" s="2" t="n">
-        <v>6.75891868705208</v>
-      </c>
-      <c r="H29" s="2" t="n">
+      <c r="K29" s="2" t="n">
+        <v>2.04454929463239</v>
+      </c>
+      <c r="L29" s="2" t="n">
         <v>6.00636363636364</v>
       </c>
-      <c r="I29" s="2" t="n">
+      <c r="M29" s="2" t="n">
         <v>3.19619233691364</v>
       </c>
-      <c r="J29" s="2" t="n">
+      <c r="N29" s="2" t="n">
         <v>9.61909090909091</v>
       </c>
-      <c r="K29" s="2" t="n">
+      <c r="O29" s="2" t="n">
         <v>5.96558539381586</v>
       </c>
-      <c r="L29" s="2" t="n">
+      <c r="P29" s="2" t="n">
         <v>-1.43545685290696</v>
       </c>
-      <c r="M29" s="2" t="n">
+      <c r="Q29" s="2" t="n">
         <v>0.57045903454402</v>
       </c>
-      <c r="N29" s="2" t="n">
+      <c r="R29" s="2" t="n">
         <v>-0.436606631640276</v>
       </c>
-      <c r="O29" s="2" t="n">
+      <c r="S29" s="2" t="n">
         <v>0.530208692413226</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>7</v>
       </c>
       <c r="D30" s="2" t="n">
+        <v>446</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>558</v>
+      </c>
+      <c r="F30" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G30" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H30" s="2" t="n">
         <v>19.2616666666667</v>
       </c>
-      <c r="E30" s="2" t="n">
-        <v>12.7152167369128</v>
-      </c>
-      <c r="F30" s="2" t="n">
+      <c r="I30" s="2" t="n">
+        <v>2.28543868874227</v>
+      </c>
+      <c r="J30" s="2" t="n">
         <v>19.2116666666667</v>
       </c>
-      <c r="G30" s="2" t="n">
-        <v>13.0137195554025</v>
-      </c>
-      <c r="H30" s="2" t="n">
+      <c r="K30" s="2" t="n">
+        <v>2.15453011118434</v>
+      </c>
+      <c r="L30" s="2" t="n">
         <v>10.918</v>
       </c>
-      <c r="I30" s="2" t="n">
+      <c r="M30" s="2" t="n">
         <v>8.0430510380079</v>
       </c>
-      <c r="J30" s="2" t="n">
+      <c r="N30" s="2" t="n">
         <v>11.648</v>
       </c>
-      <c r="K30" s="2" t="n">
+      <c r="O30" s="2" t="n">
         <v>8.88954835748138</v>
       </c>
-      <c r="L30" s="2" t="n">
+      <c r="P30" s="2" t="n">
         <v>-1.8191123355899</v>
       </c>
-      <c r="M30" s="2" t="n">
+      <c r="Q30" s="2" t="n">
         <v>0.584131282761524</v>
       </c>
-      <c r="N30" s="2" t="n">
+      <c r="R30" s="2" t="n">
         <v>-1.60978882913806</v>
       </c>
-      <c r="O30" s="2" t="n">
+      <c r="S30" s="2" t="n">
         <v>0.633880045738904</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>6</v>
       </c>
       <c r="D31" s="2" t="n">
+        <v>395</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>405</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="H31" s="2" t="n">
         <v>1.812</v>
       </c>
-      <c r="E31" s="2" t="n">
-        <v>0.337298087750286</v>
-      </c>
-      <c r="F31" s="2" t="n">
+      <c r="I31" s="2" t="n">
+        <v>0.651060673055899</v>
+      </c>
+      <c r="J31" s="2" t="n">
         <v>1.816</v>
       </c>
-      <c r="G31" s="2" t="n">
-        <v>0.326006134911599</v>
-      </c>
-      <c r="H31" s="2" t="n">
+      <c r="K31" s="2" t="n">
+        <v>0.396635853144922</v>
+      </c>
+      <c r="L31" s="2" t="n">
         <v>1.43</v>
       </c>
-      <c r="I31" s="2" t="n">
+      <c r="M31" s="2" t="n">
         <v>0.255342906696074</v>
       </c>
-      <c r="J31" s="2" t="n">
+      <c r="N31" s="2" t="n">
         <v>1.8</v>
       </c>
-      <c r="K31" s="2" t="n">
+      <c r="O31" s="2" t="n">
         <v>0.346410161513775</v>
       </c>
-      <c r="L31" s="2" t="n">
+      <c r="P31" s="2" t="n">
         <v>-0.529622019771274</v>
       </c>
-      <c r="M31" s="2" t="n">
+      <c r="Q31" s="2" t="n">
         <v>0.450140214151255</v>
       </c>
-      <c r="N31" s="2" t="n">
+      <c r="R31" s="2" t="n">
         <v>-0.108051948051948</v>
       </c>
-      <c r="O31" s="2" t="n">
+      <c r="S31" s="2" t="n">
         <v>0.281744958269162</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D32" s="2" t="n">
+        <v>492</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>583</v>
+      </c>
+      <c r="F32" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G32" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H32" s="2" t="n">
         <v>25.775</v>
       </c>
-      <c r="E32" s="2" t="n">
-        <v>3.43159341025905</v>
-      </c>
-      <c r="F32" s="2" t="n">
+      <c r="I32" s="2" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="J32" s="2" t="n">
         <v>25.625</v>
       </c>
-      <c r="G32" s="2" t="n">
-        <v>3.48843326819744</v>
-      </c>
-      <c r="H32" s="2" t="n">
+      <c r="K32" s="2" t="n">
+        <v>1.27541823205828</v>
+      </c>
+      <c r="L32" s="2" t="n">
         <v>11.2</v>
-      </c>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2" t="n">
-        <v>13.9</v>
-      </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2" t="n">
-        <v>-1.26060606060606</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2" t="n">
+        <v>-1.26060606060606</v>
+      </c>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2" t="n">
         <v>-0.921212121212121</v>
       </c>
-      <c r="O32" s="2"/>
+      <c r="S32" s="2"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D33" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E33" s="2"/>
+      <c r="D33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F33" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G33" s="2"/>
+      <c r="G33" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H33" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1833,25 +2233,37 @@
         <v>#NUM!</v>
       </c>
       <c r="O33" s="2"/>
+      <c r="P33" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S33" s="2"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D34" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E34" s="2"/>
+      <c r="D34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F34" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G34" s="2"/>
+      <c r="G34" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H34" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1868,72 +2280,96 @@
         <v>#NUM!</v>
       </c>
       <c r="O34" s="2"/>
+      <c r="P34" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S34" s="2"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D35" s="2" t="n">
+        <v>866</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>978</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>14.16</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>14.16</v>
+      </c>
+      <c r="H35" s="2" t="n">
         <v>22.3822222222222</v>
       </c>
-      <c r="E35" s="2" t="n">
-        <v>10.0646271388683</v>
-      </c>
-      <c r="F35" s="2" t="n">
+      <c r="I35" s="2" t="n">
+        <v>3.22900526478357</v>
+      </c>
+      <c r="J35" s="2" t="n">
         <v>22.4644444444444</v>
       </c>
-      <c r="G35" s="2" t="n">
-        <v>10.2677262710776</v>
-      </c>
-      <c r="H35" s="2" t="n">
+      <c r="K35" s="2" t="n">
+        <v>4.14688571232812</v>
+      </c>
+      <c r="L35" s="2" t="n">
         <v>14.5122222222222</v>
       </c>
-      <c r="I35" s="2" t="n">
+      <c r="M35" s="2" t="n">
         <v>7.76139288043354</v>
       </c>
-      <c r="J35" s="2" t="n">
+      <c r="N35" s="2" t="n">
         <v>17.0688888888889</v>
       </c>
-      <c r="K35" s="2" t="n">
+      <c r="O35" s="2" t="n">
         <v>8.17483554030973</v>
       </c>
-      <c r="L35" s="2" t="n">
+      <c r="P35" s="2" t="n">
         <v>-0.895854408619479</v>
       </c>
-      <c r="M35" s="2" t="n">
+      <c r="Q35" s="2" t="n">
         <v>0.563701596552756</v>
       </c>
-      <c r="N35" s="2" t="n">
+      <c r="R35" s="2" t="n">
         <v>-0.512728027527365</v>
       </c>
-      <c r="O35" s="2" t="n">
+      <c r="S35" s="2" t="n">
         <v>0.280797119470041</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D36" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E36" s="2"/>
+      <c r="D36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F36" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H36" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1950,60 +2386,84 @@
         <v>#NUM!</v>
       </c>
       <c r="O36" s="2"/>
+      <c r="P36" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S36" s="2"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D37" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>4.349</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>4.349</v>
+      </c>
+      <c r="H37" s="2" t="n">
         <v>11.3</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2" t="n">
-        <v>7.6</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2" t="n">
-        <v>7.5</v>
+        <v>9</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2" t="n">
-        <v>-0.902439024390244</v>
+        <v>7.6</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2" t="n">
+        <v>-0.902439024390244</v>
+      </c>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2" t="n">
         <v>-0.319148936170213</v>
       </c>
-      <c r="O37" s="2"/>
+      <c r="S37" s="2"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D38" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E38" s="2"/>
+      <c r="D38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F38" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G38" s="2"/>
+      <c r="G38" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H38" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2020,60 +2480,84 @@
         <v>#NUM!</v>
       </c>
       <c r="O38" s="2"/>
+      <c r="P38" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S38" s="2"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D39" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>4.349</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>4.349</v>
+      </c>
+      <c r="H39" s="2" t="n">
         <v>42.8</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2" t="n">
-        <v>39.8</v>
-      </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2" t="n">
-        <v>30.1</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="n">
-        <v>33.7</v>
+        <v>39.8</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2" t="n">
-        <v>-1.48538011695906</v>
+        <v>30.1</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2" t="n">
+        <v>-1.48538011695906</v>
+      </c>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2" t="n">
         <v>-0.583732057416267</v>
       </c>
-      <c r="O39" s="2"/>
+      <c r="S39" s="2"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D40" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E40" s="2"/>
+      <c r="D40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F40" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G40" s="2"/>
+      <c r="G40" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H40" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2090,133 +2574,177 @@
         <v>#NUM!</v>
       </c>
       <c r="O40" s="2"/>
+      <c r="P40" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S40" s="2"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D41" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>16.37</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>16.37</v>
+      </c>
+      <c r="H41" s="2" t="n">
         <v>12.22</v>
       </c>
-      <c r="E41" s="2" t="n">
-        <v>4.21435641587182</v>
-      </c>
-      <c r="F41" s="2" t="n">
+      <c r="I41" s="2" t="n">
+        <v>0.127279220613578</v>
+      </c>
+      <c r="J41" s="2" t="n">
         <v>13.41</v>
       </c>
-      <c r="G41" s="2" t="n">
-        <v>2.10717820793591</v>
-      </c>
-      <c r="H41" s="2" t="n">
+      <c r="K41" s="2" t="n">
+        <v>1.32228968081884</v>
+      </c>
+      <c r="L41" s="2" t="n">
         <v>7.77</v>
       </c>
-      <c r="I41" s="2" t="n">
+      <c r="M41" s="2" t="n">
         <v>2.72943217538007</v>
       </c>
-      <c r="J41" s="2" t="n">
+      <c r="N41" s="2" t="n">
         <v>10.62</v>
       </c>
-      <c r="K41" s="2" t="n">
+      <c r="O41" s="2" t="n">
         <v>0.254558441227158</v>
       </c>
-      <c r="L41" s="2" t="n">
+      <c r="P41" s="2" t="n">
         <v>-1.12098427887902</v>
       </c>
-      <c r="M41" s="2" t="n">
+      <c r="Q41" s="2" t="n">
         <v>0.434993918706694</v>
       </c>
-      <c r="N41" s="2" t="n">
+      <c r="R41" s="2" t="n">
         <v>-0.62504752851711</v>
       </c>
-      <c r="O41" s="2" t="n">
+      <c r="S41" s="2" t="n">
         <v>0.565618209475741</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D42" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="F42" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G42" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H42" s="2" t="n">
         <v>76.96</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2" t="n">
-        <v>81.26</v>
-      </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2" t="n">
-        <v>60.58</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2" t="n">
-        <v>66.68</v>
+        <v>81.26</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2" t="n">
-        <v>-1.4469964664311</v>
+        <v>60.58</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2" t="n">
+        <v>66.68</v>
+      </c>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2" t="n">
+        <v>-1.4469964664311</v>
+      </c>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2" t="n">
         <v>-1.4134755210858</v>
       </c>
-      <c r="O42" s="2"/>
+      <c r="S42" s="2"/>
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C43" s="3" t="n">
         <v>7</v>
       </c>
       <c r="D43" s="3" t="n">
+        <v>199</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>196</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>14.0285714285714</v>
+      </c>
+      <c r="G43" s="3" t="n">
+        <v>14.0285714285714</v>
+      </c>
+      <c r="H43" s="3" t="n">
         <v>84.28</v>
       </c>
-      <c r="E43" s="3" t="n">
-        <v>3.37123122909124</v>
-      </c>
-      <c r="F43" s="3" t="n">
+      <c r="I43" s="3" t="n">
+        <v>1.03538237703115</v>
+      </c>
+      <c r="J43" s="3" t="n">
         <v>82.7183333333333</v>
       </c>
-      <c r="G43" s="3" t="n">
-        <v>2.37147563062888</v>
-      </c>
-      <c r="H43" s="3" t="n">
+      <c r="K43" s="3" t="n">
+        <v>2.8028033585442</v>
+      </c>
+      <c r="L43" s="3" t="n">
         <v>61.74</v>
       </c>
-      <c r="I43" s="3" t="n">
+      <c r="M43" s="3" t="n">
         <v>6.73220320548927</v>
       </c>
-      <c r="J43" s="3" t="n">
+      <c r="N43" s="3" t="n">
         <v>72.6</v>
       </c>
-      <c r="K43" s="3" t="n">
+      <c r="O43" s="3" t="n">
         <v>8.76907292705449</v>
       </c>
-      <c r="L43" s="3" t="n">
+      <c r="P43" s="3" t="n">
         <v>-2.17171639105173</v>
       </c>
-      <c r="M43" s="3" t="n">
+      <c r="Q43" s="3" t="n">
         <v>0.758232949400711</v>
       </c>
-      <c r="N43" s="3" t="n">
+      <c r="R43" s="3" t="n">
         <v>-0.976005277885888</v>
       </c>
-      <c r="O43" s="3" t="n">
+      <c r="S43" s="3" t="n">
         <v>0.805622084947634</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Having problems with my git, hoping this will fix merge errors
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t xml:space="preserve">instr</t>
   </si>
@@ -21,6 +21,18 @@
   </si>
   <si>
     <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_n_control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total_n_active</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg_active_age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">avg_control_age</t>
   </si>
   <si>
     <t xml:space="preserve">avg_baseline_mean_act</t>
@@ -541,25 +553,41 @@
       <c r="O1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0</v>
+      </c>
       <c r="F2" s="1" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H2" s="1" t="e">
         <v>#NUM!</v>
       </c>
@@ -576,25 +604,37 @@
         <v>#NUM!</v>
       </c>
       <c r="O2" s="1"/>
+      <c r="P2" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="D3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F3" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H3" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -611,25 +651,37 @@
         <v>#NUM!</v>
       </c>
       <c r="O3" s="2"/>
+      <c r="P3" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="D4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F4" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H4" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -646,166 +698,214 @@
         <v>#NUM!</v>
       </c>
       <c r="O4" s="2"/>
+      <c r="P4" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D5" s="2" t="n">
+        <v>209</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>210</v>
+      </c>
+      <c r="F5" s="2" t="n">
+        <v>14.97</v>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>14.97</v>
+      </c>
+      <c r="H5" s="2" t="n">
         <v>43.5</v>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="n">
+      <c r="I5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
         <v>44.2</v>
       </c>
-      <c r="G5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="n">
+      <c r="K5" s="2" t="n">
+        <v>0.282842712474618</v>
+      </c>
+      <c r="L5" s="2" t="n">
         <v>27.8</v>
       </c>
-      <c r="I5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2" t="n">
+      <c r="M5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2" t="n">
         <v>38.95</v>
       </c>
-      <c r="K5" s="2" t="n">
+      <c r="O5" s="2" t="n">
         <v>2.33345237791561</v>
       </c>
-      <c r="L5" s="2" t="n">
+      <c r="P5" s="2" t="n">
         <v>-1.15018315018315</v>
       </c>
-      <c r="M5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2" t="n">
+      <c r="Q5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2" t="n">
         <v>-0.392255962574663</v>
       </c>
-      <c r="O5" s="2" t="n">
+      <c r="S5" s="2" t="n">
         <v>0.176208139031742</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D6" s="2" t="n">
+        <v>161</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>253</v>
+      </c>
+      <c r="F6" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G6" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H6" s="2" t="n">
         <v>21.6066666666667</v>
       </c>
-      <c r="E6" s="2" t="n">
-        <v>3.90129892898934</v>
-      </c>
-      <c r="F6" s="2" t="n">
+      <c r="I6" s="2" t="n">
+        <v>1.895793589327</v>
+      </c>
+      <c r="J6" s="2" t="n">
         <v>18.99</v>
       </c>
-      <c r="G6" s="2" t="n">
-        <v>5.20406571826298</v>
-      </c>
-      <c r="H6" s="2" t="n">
+      <c r="K6" s="2" t="n">
+        <v>1.16988603433554</v>
+      </c>
+      <c r="L6" s="2" t="n">
         <v>10.9733333333333</v>
       </c>
-      <c r="I6" s="2" t="n">
+      <c r="M6" s="2" t="n">
         <v>2.9759256263108</v>
       </c>
-      <c r="J6" s="2" t="n">
+      <c r="N6" s="2" t="n">
         <v>13.7466666666667</v>
       </c>
-      <c r="K6" s="2" t="n">
+      <c r="O6" s="2" t="n">
         <v>4.91468547654205</v>
       </c>
-      <c r="L6" s="2" t="n">
+      <c r="P6" s="2" t="n">
         <v>-1.12611988022129</v>
       </c>
-      <c r="M6" s="2" t="n">
+      <c r="Q6" s="2" t="n">
         <v>0.286097061706614</v>
       </c>
-      <c r="N6" s="2" t="n">
+      <c r="R6" s="2" t="n">
         <v>-0.506105006105006</v>
       </c>
-      <c r="O6" s="2" t="n">
+      <c r="S6" s="2" t="n">
         <v>0.0562697385464052</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>20</v>
       </c>
       <c r="D7" s="2" t="n">
+        <v>658</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>679</v>
+      </c>
+      <c r="F7" s="2" t="n">
+        <v>15.8975</v>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>15.8975</v>
+      </c>
+      <c r="H7" s="2" t="n">
         <v>23.6705</v>
       </c>
-      <c r="E7" s="2" t="n">
-        <v>6.52625747108918</v>
-      </c>
-      <c r="F7" s="2" t="n">
+      <c r="I7" s="2" t="n">
+        <v>2.65185257985114</v>
+      </c>
+      <c r="J7" s="2" t="n">
         <v>22.9795</v>
       </c>
-      <c r="G7" s="2" t="n">
-        <v>6.85459237146509</v>
-      </c>
-      <c r="H7" s="2" t="n">
+      <c r="K7" s="2" t="n">
+        <v>2.75376278457027</v>
+      </c>
+      <c r="L7" s="2" t="n">
         <v>11.7575</v>
       </c>
-      <c r="I7" s="2" t="n">
+      <c r="M7" s="2" t="n">
         <v>5.00914518918306</v>
       </c>
-      <c r="J7" s="2" t="n">
+      <c r="N7" s="2" t="n">
         <v>17.8565</v>
       </c>
-      <c r="K7" s="2" t="n">
+      <c r="O7" s="2" t="n">
         <v>6.6560920057849</v>
       </c>
-      <c r="L7" s="2" t="n">
+      <c r="P7" s="2" t="n">
         <v>-1.63100033703923</v>
       </c>
-      <c r="M7" s="2" t="n">
+      <c r="Q7" s="2" t="n">
         <v>1.31802595898147</v>
       </c>
-      <c r="N7" s="2" t="n">
+      <c r="R7" s="2" t="n">
         <v>-0.601378145829666</v>
       </c>
-      <c r="O7" s="2" t="n">
+      <c r="S7" s="2" t="n">
         <v>0.625188776821564</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D8" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E8" s="2"/>
+      <c r="D8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F8" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H8" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -822,72 +922,96 @@
         <v>#NUM!</v>
       </c>
       <c r="O8" s="2"/>
+      <c r="P8" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>5</v>
       </c>
       <c r="D9" s="2" t="n">
+        <v>72</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>69</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>13.54</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>13.54</v>
+      </c>
+      <c r="H9" s="2" t="n">
         <v>48.556</v>
       </c>
-      <c r="E9" s="2" t="n">
-        <v>3.70774594598929</v>
-      </c>
-      <c r="F9" s="2" t="n">
+      <c r="I9" s="2" t="n">
+        <v>2.0571290674141</v>
+      </c>
+      <c r="J9" s="2" t="n">
         <v>41.374</v>
       </c>
-      <c r="G9" s="2" t="n">
-        <v>3.84551426989941</v>
-      </c>
-      <c r="H9" s="2" t="n">
+      <c r="K9" s="2" t="n">
+        <v>3.21606902910992</v>
+      </c>
+      <c r="L9" s="2" t="n">
         <v>16.178</v>
       </c>
-      <c r="I9" s="2" t="n">
+      <c r="M9" s="2" t="n">
         <v>0.808498608533125</v>
       </c>
-      <c r="J9" s="2" t="n">
+      <c r="N9" s="2" t="n">
         <v>30.078</v>
       </c>
-      <c r="K9" s="2" t="n">
+      <c r="O9" s="2" t="n">
         <v>13.4953147425319</v>
       </c>
-      <c r="L9" s="2" t="n">
+      <c r="P9" s="2" t="n">
         <v>-2.06506081209349</v>
       </c>
-      <c r="M9" s="2" t="n">
+      <c r="Q9" s="2" t="n">
         <v>0.218537778971517</v>
       </c>
-      <c r="N9" s="2" t="n">
+      <c r="R9" s="2" t="n">
         <v>-0.659844596408108</v>
       </c>
-      <c r="O9" s="2" t="n">
+      <c r="S9" s="2" t="n">
         <v>1.06191966398227</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D10" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E10" s="2"/>
+      <c r="D10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F10" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H10" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -904,72 +1028,96 @@
         <v>#NUM!</v>
       </c>
       <c r="O10" s="2"/>
+      <c r="P10" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D11" s="2" t="n">
+        <v>216</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>226</v>
+      </c>
+      <c r="F11" s="2" t="n">
+        <v>14.7822222222222</v>
+      </c>
+      <c r="G11" s="2" t="n">
+        <v>14.7822222222222</v>
+      </c>
+      <c r="H11" s="2" t="n">
         <v>32.1544444444444</v>
       </c>
-      <c r="E11" s="2" t="n">
-        <v>29.3985739922497</v>
-      </c>
-      <c r="F11" s="2" t="n">
+      <c r="I11" s="2" t="n">
+        <v>2.20080730137324</v>
+      </c>
+      <c r="J11" s="2" t="n">
         <v>30.0533333333333</v>
       </c>
-      <c r="G11" s="2" t="n">
-        <v>27.3780605595064</v>
-      </c>
-      <c r="H11" s="2" t="n">
+      <c r="K11" s="2" t="n">
+        <v>2.83738337988444</v>
+      </c>
+      <c r="L11" s="2" t="n">
         <v>27.6433333333333</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="M11" s="2" t="n">
         <v>28.1645703855038</v>
       </c>
-      <c r="J11" s="2" t="n">
+      <c r="N11" s="2" t="n">
         <v>28.2955555555556</v>
       </c>
-      <c r="K11" s="2" t="n">
+      <c r="O11" s="2" t="n">
         <v>29.9785648885629</v>
       </c>
-      <c r="L11" s="2" t="n">
+      <c r="P11" s="2" t="n">
         <v>-0.766537651364512</v>
       </c>
-      <c r="M11" s="2" t="n">
+      <c r="Q11" s="2" t="n">
         <v>0.738100761848697</v>
       </c>
-      <c r="N11" s="2" t="n">
+      <c r="R11" s="2" t="n">
         <v>-0.413957059870753</v>
       </c>
-      <c r="O11" s="2" t="n">
+      <c r="S11" s="2" t="n">
         <v>0.595212113379861</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D12" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E12" s="2"/>
+      <c r="D12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F12" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H12" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -986,166 +1134,214 @@
         <v>#NUM!</v>
       </c>
       <c r="O12" s="2"/>
+      <c r="P12" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>23</v>
       </c>
       <c r="D13" s="2" t="n">
+        <v>804</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>826</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>12.5977272727273</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>12.5977272727273</v>
+      </c>
+      <c r="H13" s="2" t="n">
         <v>21.7127272727273</v>
       </c>
-      <c r="E13" s="2" t="n">
-        <v>5.83141997068114</v>
-      </c>
-      <c r="F13" s="2" t="n">
+      <c r="I13" s="2" t="n">
+        <v>1.84699562997395</v>
+      </c>
+      <c r="J13" s="2" t="n">
         <v>20.3345454545455</v>
       </c>
-      <c r="G13" s="2" t="n">
-        <v>6.28488112345259</v>
-      </c>
-      <c r="H13" s="2" t="n">
+      <c r="K13" s="2" t="n">
+        <v>2.58903484498981</v>
+      </c>
+      <c r="L13" s="2" t="n">
         <v>12.0717391304348</v>
       </c>
-      <c r="I13" s="2" t="n">
+      <c r="M13" s="2" t="n">
         <v>3.85507888396347</v>
       </c>
-      <c r="J13" s="2" t="n">
+      <c r="N13" s="2" t="n">
         <v>16.9395652173913</v>
       </c>
-      <c r="K13" s="2" t="n">
+      <c r="O13" s="2" t="n">
         <v>5.6824670364687</v>
       </c>
-      <c r="L13" s="2" t="n">
+      <c r="P13" s="2" t="n">
         <v>-1.15683202443842</v>
       </c>
-      <c r="M13" s="2" t="n">
+      <c r="Q13" s="2" t="n">
         <v>0.616974044793137</v>
       </c>
-      <c r="N13" s="2" t="n">
+      <c r="R13" s="2" t="n">
         <v>-0.380298979613213</v>
       </c>
-      <c r="O13" s="2" t="n">
+      <c r="S13" s="2" t="n">
         <v>0.680937833475856</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>26</v>
       </c>
       <c r="D14" s="2" t="n">
+        <v>2049</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>2128</v>
+      </c>
+      <c r="F14" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G14" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H14" s="2" t="n">
         <v>57.5021052631579</v>
       </c>
-      <c r="E14" s="2" t="n">
-        <v>3.52352030243015</v>
-      </c>
-      <c r="F14" s="2" t="n">
+      <c r="I14" s="2" t="n">
+        <v>2.60477491944167</v>
+      </c>
+      <c r="J14" s="2" t="n">
         <v>57.4957894736842</v>
       </c>
-      <c r="G14" s="2" t="n">
-        <v>3.54585566509141</v>
-      </c>
-      <c r="H14" s="2" t="n">
+      <c r="K14" s="2" t="n">
+        <v>2.72964623558229</v>
+      </c>
+      <c r="L14" s="2" t="n">
         <v>35.1913333333333</v>
       </c>
-      <c r="I14" s="2" t="n">
+      <c r="M14" s="2" t="n">
         <v>1.3935917964878</v>
       </c>
-      <c r="J14" s="2" t="n">
+      <c r="N14" s="2" t="n">
         <v>37.412</v>
       </c>
-      <c r="K14" s="2" t="n">
+      <c r="O14" s="2" t="n">
         <v>3.87342631639888</v>
       </c>
-      <c r="L14" s="2" t="n">
+      <c r="P14" s="2" t="n">
         <v>-2.2756000958178</v>
       </c>
-      <c r="M14" s="2" t="n">
+      <c r="Q14" s="2" t="n">
         <v>0.826862337778918</v>
       </c>
-      <c r="N14" s="2" t="n">
+      <c r="R14" s="2" t="n">
         <v>-1.96011632040328</v>
       </c>
-      <c r="O14" s="2" t="n">
+      <c r="S14" s="2" t="n">
         <v>0.875318084876132</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>8</v>
       </c>
       <c r="D15" s="2" t="n">
+        <v>215</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>201</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>13.80375</v>
+      </c>
+      <c r="G15" s="2" t="n">
+        <v>13.80375</v>
+      </c>
+      <c r="H15" s="2" t="n">
         <v>47.8928571428571</v>
       </c>
-      <c r="E15" s="2" t="n">
-        <v>12.253269923148</v>
-      </c>
-      <c r="F15" s="2" t="n">
+      <c r="I15" s="2" t="n">
+        <v>4.1924643281556</v>
+      </c>
+      <c r="J15" s="2" t="n">
         <v>45.1657142857143</v>
       </c>
-      <c r="G15" s="2" t="n">
-        <v>14.2387614830584</v>
-      </c>
-      <c r="H15" s="2" t="n">
+      <c r="K15" s="2" t="n">
+        <v>3.54110959204275</v>
+      </c>
+      <c r="L15" s="2" t="n">
         <v>32.4457142857143</v>
       </c>
-      <c r="I15" s="2" t="n">
+      <c r="M15" s="2" t="n">
         <v>7.47242454437839</v>
       </c>
-      <c r="J15" s="2" t="n">
+      <c r="N15" s="2" t="n">
         <v>35.0257142857143</v>
       </c>
-      <c r="K15" s="2" t="n">
+      <c r="O15" s="2" t="n">
         <v>6.61467776273054</v>
       </c>
-      <c r="L15" s="2" t="n">
+      <c r="P15" s="2" t="n">
         <v>-1.98483574563368</v>
       </c>
-      <c r="M15" s="2" t="n">
+      <c r="Q15" s="2" t="n">
         <v>1.38937759873451</v>
       </c>
-      <c r="N15" s="2" t="n">
+      <c r="R15" s="2" t="n">
         <v>-1.39269623963861</v>
       </c>
-      <c r="O15" s="2" t="n">
+      <c r="S15" s="2" t="n">
         <v>1.30755814489424</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D16" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E16" s="2"/>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F16" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H16" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1162,72 +1358,96 @@
         <v>#NUM!</v>
       </c>
       <c r="O16" s="2"/>
+      <c r="P16" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D17" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>11.17</v>
+      </c>
+      <c r="G17" s="2" t="n">
+        <v>11.17</v>
+      </c>
+      <c r="H17" s="2" t="n">
         <v>71.75</v>
       </c>
-      <c r="E17" s="2" t="n">
-        <v>0.91923881554252</v>
-      </c>
-      <c r="F17" s="2" t="n">
+      <c r="I17" s="2" t="n">
+        <v>0.0494974746830585</v>
+      </c>
+      <c r="J17" s="2" t="n">
         <v>67.56</v>
       </c>
-      <c r="G17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H17" s="2" t="n">
+      <c r="K17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L17" s="2" t="n">
         <v>52.62</v>
       </c>
-      <c r="I17" s="2" t="n">
+      <c r="M17" s="2" t="n">
         <v>3.50724963468528</v>
       </c>
-      <c r="J17" s="2" t="n">
+      <c r="N17" s="2" t="n">
         <v>61.09</v>
       </c>
-      <c r="K17" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L17" s="2" t="n">
+      <c r="O17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P17" s="2" t="n">
         <v>-1.88141575073107</v>
       </c>
-      <c r="M17" s="2" t="n">
+      <c r="Q17" s="2" t="n">
         <v>0.654746986929079</v>
       </c>
-      <c r="N17" s="2" t="n">
+      <c r="R17" s="2" t="n">
         <v>-0.374746597161888</v>
       </c>
-      <c r="O17" s="2" t="n">
+      <c r="S17" s="2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D18" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E18" s="2"/>
+      <c r="D18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F18" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H18" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1244,72 +1464,96 @@
         <v>#NUM!</v>
       </c>
       <c r="O18" s="2"/>
+      <c r="P18" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S18" s="2"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>13</v>
       </c>
       <c r="D19" s="2" t="n">
+        <v>509</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>541</v>
+      </c>
+      <c r="F19" s="2" t="n">
+        <v>15.4653846153846</v>
+      </c>
+      <c r="G19" s="2" t="n">
+        <v>15.4653846153846</v>
+      </c>
+      <c r="H19" s="2" t="n">
         <v>22.1481818181818</v>
       </c>
-      <c r="E19" s="2" t="n">
-        <v>7.39583101237693</v>
-      </c>
-      <c r="F19" s="2" t="n">
+      <c r="I19" s="2" t="n">
+        <v>2.13475993966535</v>
+      </c>
+      <c r="J19" s="2" t="n">
         <v>22.3363636363636</v>
       </c>
-      <c r="G19" s="2" t="n">
-        <v>7.11567744171596</v>
-      </c>
-      <c r="H19" s="2" t="n">
+      <c r="K19" s="2" t="n">
+        <v>3.46703174068382</v>
+      </c>
+      <c r="L19" s="2" t="n">
         <v>14.6654545454545</v>
       </c>
-      <c r="I19" s="2" t="n">
+      <c r="M19" s="2" t="n">
         <v>7.5560483900467</v>
       </c>
-      <c r="J19" s="2" t="n">
+      <c r="N19" s="2" t="n">
         <v>19.6636363636364</v>
       </c>
-      <c r="K19" s="2" t="n">
+      <c r="O19" s="2" t="n">
         <v>6.29988773348744</v>
       </c>
-      <c r="L19" s="2" t="n">
+      <c r="P19" s="2" t="n">
         <v>-1.02786088724732</v>
       </c>
-      <c r="M19" s="2" t="n">
+      <c r="Q19" s="2" t="n">
         <v>0.717959167358529</v>
       </c>
-      <c r="N19" s="2" t="n">
+      <c r="R19" s="2" t="n">
         <v>-0.315175193070365</v>
       </c>
-      <c r="O19" s="2" t="n">
+      <c r="S19" s="2" t="n">
         <v>0.323783853617054</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="D20" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E20" s="2"/>
+      <c r="D20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F20" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G20" s="2"/>
+      <c r="G20" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H20" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1326,25 +1570,37 @@
         <v>#NUM!</v>
       </c>
       <c r="O20" s="2"/>
+      <c r="P20" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S20" s="2"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D21" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E21" s="2"/>
+      <c r="D21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F21" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H21" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1361,25 +1617,37 @@
         <v>#NUM!</v>
       </c>
       <c r="O21" s="2"/>
+      <c r="P21" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S21" s="2"/>
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D22" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E22" s="2"/>
+      <c r="D22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F22" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H22" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1396,60 +1664,84 @@
         <v>#NUM!</v>
       </c>
       <c r="O22" s="2"/>
+      <c r="P22" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S22" s="2"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="E23" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="F23" s="2" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="G23" s="2" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="H23" s="2" t="n">
         <v>24.2</v>
-      </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="n">
-        <v>21.6</v>
-      </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2" t="n">
-        <v>17.2</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2" t="n">
-        <v>23.93</v>
+        <v>21.6</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2" t="n">
-        <v>-0.78125</v>
+        <v>17.2</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2" t="n">
+        <v>23.93</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2" t="n">
+        <v>-0.78125</v>
+      </c>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2" t="n">
         <v>0.20610349402919</v>
       </c>
-      <c r="O23" s="2"/>
+      <c r="S23" s="2"/>
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D24" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E24" s="2"/>
+      <c r="D24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F24" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G24" s="2"/>
+      <c r="G24" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H24" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1466,95 +1758,131 @@
         <v>#NUM!</v>
       </c>
       <c r="O24" s="2"/>
+      <c r="P24" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S24" s="2"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E25" s="2" t="n">
+        <v>32</v>
+      </c>
+      <c r="F25" s="2" t="n">
+        <v>11.77</v>
+      </c>
+      <c r="G25" s="2" t="n">
+        <v>11.77</v>
+      </c>
+      <c r="H25" s="2" t="n">
         <v>10.44</v>
-      </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2" t="n">
-        <v>11.33</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2" t="n">
-        <v>5.13</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2" t="n">
-        <v>6.65</v>
+        <v>11.33</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2" t="n">
-        <v>-1.18791946308725</v>
+        <v>5.13</v>
       </c>
       <c r="M25" s="2"/>
       <c r="N25" s="2" t="n">
+        <v>6.65</v>
+      </c>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2" t="n">
+        <v>-1.18791946308725</v>
+      </c>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2" t="n">
         <v>-1.00970873786408</v>
       </c>
-      <c r="O25" s="2"/>
+      <c r="S25" s="2"/>
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="F26" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G26" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H26" s="2" t="n">
         <v>37.6</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2" t="n">
-        <v>38.6</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2" t="n">
-        <v>54.2</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2" t="n">
-        <v>48.9</v>
+        <v>38.6</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2" t="n">
-        <v>1.77540106951872</v>
+        <v>54.2</v>
       </c>
       <c r="M26" s="2"/>
       <c r="N26" s="2" t="n">
+        <v>48.9</v>
+      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2" t="n">
+        <v>1.77540106951872</v>
+      </c>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="2" t="n">
         <v>1.02487562189055</v>
       </c>
-      <c r="O26" s="2"/>
+      <c r="S26" s="2"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D27" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E27" s="2"/>
+      <c r="D27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F27" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H27" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1571,252 +1899,324 @@
         <v>#NUM!</v>
       </c>
       <c r="O27" s="2"/>
+      <c r="P27" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S27" s="2"/>
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>9</v>
       </c>
       <c r="D28" s="2" t="n">
+        <v>438</v>
+      </c>
+      <c r="E28" s="2" t="n">
+        <v>457</v>
+      </c>
+      <c r="F28" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G28" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H28" s="2" t="n">
         <v>19.1414285714286</v>
       </c>
-      <c r="E28" s="2" t="n">
-        <v>3.71034332899903</v>
-      </c>
-      <c r="F28" s="2" t="n">
+      <c r="I28" s="2" t="n">
+        <v>0.68668284770579</v>
+      </c>
+      <c r="J28" s="2" t="n">
         <v>19.73</v>
       </c>
-      <c r="G28" s="2" t="n">
-        <v>3.68908751138634</v>
-      </c>
-      <c r="H28" s="2" t="n">
+      <c r="K28" s="2" t="n">
+        <v>0.681682093200692</v>
+      </c>
+      <c r="L28" s="2" t="n">
         <v>10.1716666666667</v>
       </c>
-      <c r="I28" s="2" t="n">
+      <c r="M28" s="2" t="n">
         <v>2.09659167857422</v>
       </c>
-      <c r="J28" s="2" t="n">
+      <c r="N28" s="2" t="n">
         <v>11.6683333333333</v>
       </c>
-      <c r="K28" s="2" t="n">
+      <c r="O28" s="2" t="n">
         <v>2.42543535610963</v>
       </c>
-      <c r="L28" s="2" t="n">
+      <c r="P28" s="2" t="n">
         <v>-1.81433607742254</v>
       </c>
-      <c r="M28" s="2" t="n">
+      <c r="Q28" s="2" t="n">
         <v>1.05185624392889</v>
       </c>
-      <c r="N28" s="2" t="n">
+      <c r="R28" s="2" t="n">
         <v>-1.49139968116527</v>
       </c>
-      <c r="O28" s="2" t="n">
+      <c r="S28" s="2" t="n">
         <v>0.262979127241591</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>11</v>
       </c>
       <c r="D29" s="2" t="n">
+        <v>356</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>352</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>15.6909090909091</v>
+      </c>
+      <c r="G29" s="2" t="n">
+        <v>15.6909090909091</v>
+      </c>
+      <c r="H29" s="2" t="n">
         <v>13.2318181818182</v>
       </c>
-      <c r="E29" s="2" t="n">
-        <v>6.48560994538188</v>
-      </c>
-      <c r="F29" s="2" t="n">
+      <c r="I29" s="2" t="n">
+        <v>1.77901913730828</v>
+      </c>
+      <c r="J29" s="2" t="n">
         <v>12.4327272727273</v>
       </c>
-      <c r="G29" s="2" t="n">
-        <v>6.75891868705208</v>
-      </c>
-      <c r="H29" s="2" t="n">
+      <c r="K29" s="2" t="n">
+        <v>2.04454929463239</v>
+      </c>
+      <c r="L29" s="2" t="n">
         <v>6.00636363636364</v>
       </c>
-      <c r="I29" s="2" t="n">
+      <c r="M29" s="2" t="n">
         <v>3.19619233691364</v>
       </c>
-      <c r="J29" s="2" t="n">
+      <c r="N29" s="2" t="n">
         <v>9.61909090909091</v>
       </c>
-      <c r="K29" s="2" t="n">
+      <c r="O29" s="2" t="n">
         <v>5.96558539381586</v>
       </c>
-      <c r="L29" s="2" t="n">
+      <c r="P29" s="2" t="n">
         <v>-1.43545685290696</v>
       </c>
-      <c r="M29" s="2" t="n">
+      <c r="Q29" s="2" t="n">
         <v>0.57045903454402</v>
       </c>
-      <c r="N29" s="2" t="n">
+      <c r="R29" s="2" t="n">
         <v>-0.436606631640276</v>
       </c>
-      <c r="O29" s="2" t="n">
+      <c r="S29" s="2" t="n">
         <v>0.530208692413226</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>7</v>
       </c>
       <c r="D30" s="2" t="n">
+        <v>446</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>558</v>
+      </c>
+      <c r="F30" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G30" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H30" s="2" t="n">
         <v>19.2616666666667</v>
       </c>
-      <c r="E30" s="2" t="n">
-        <v>12.7152167369128</v>
-      </c>
-      <c r="F30" s="2" t="n">
+      <c r="I30" s="2" t="n">
+        <v>2.28543868874227</v>
+      </c>
+      <c r="J30" s="2" t="n">
         <v>19.2116666666667</v>
       </c>
-      <c r="G30" s="2" t="n">
-        <v>13.0137195554025</v>
-      </c>
-      <c r="H30" s="2" t="n">
+      <c r="K30" s="2" t="n">
+        <v>2.15453011118434</v>
+      </c>
+      <c r="L30" s="2" t="n">
         <v>10.918</v>
       </c>
-      <c r="I30" s="2" t="n">
+      <c r="M30" s="2" t="n">
         <v>8.0430510380079</v>
       </c>
-      <c r="J30" s="2" t="n">
+      <c r="N30" s="2" t="n">
         <v>11.648</v>
       </c>
-      <c r="K30" s="2" t="n">
+      <c r="O30" s="2" t="n">
         <v>8.88954835748138</v>
       </c>
-      <c r="L30" s="2" t="n">
+      <c r="P30" s="2" t="n">
         <v>-1.8191123355899</v>
       </c>
-      <c r="M30" s="2" t="n">
+      <c r="Q30" s="2" t="n">
         <v>0.584131282761524</v>
       </c>
-      <c r="N30" s="2" t="n">
+      <c r="R30" s="2" t="n">
         <v>-1.60978882913806</v>
       </c>
-      <c r="O30" s="2" t="n">
+      <c r="S30" s="2" t="n">
         <v>0.633880045738904</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>6</v>
       </c>
       <c r="D31" s="2" t="n">
+        <v>395</v>
+      </c>
+      <c r="E31" s="2" t="n">
+        <v>405</v>
+      </c>
+      <c r="F31" s="2" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="G31" s="2" t="n">
+        <v>15.65</v>
+      </c>
+      <c r="H31" s="2" t="n">
         <v>1.812</v>
       </c>
-      <c r="E31" s="2" t="n">
-        <v>0.337298087750286</v>
-      </c>
-      <c r="F31" s="2" t="n">
+      <c r="I31" s="2" t="n">
+        <v>0.651060673055899</v>
+      </c>
+      <c r="J31" s="2" t="n">
         <v>1.816</v>
       </c>
-      <c r="G31" s="2" t="n">
-        <v>0.326006134911599</v>
-      </c>
-      <c r="H31" s="2" t="n">
+      <c r="K31" s="2" t="n">
+        <v>0.396635853144922</v>
+      </c>
+      <c r="L31" s="2" t="n">
         <v>1.43</v>
       </c>
-      <c r="I31" s="2" t="n">
+      <c r="M31" s="2" t="n">
         <v>0.255342906696074</v>
       </c>
-      <c r="J31" s="2" t="n">
+      <c r="N31" s="2" t="n">
         <v>1.8</v>
       </c>
-      <c r="K31" s="2" t="n">
+      <c r="O31" s="2" t="n">
         <v>0.346410161513775</v>
       </c>
-      <c r="L31" s="2" t="n">
+      <c r="P31" s="2" t="n">
         <v>-0.529622019771274</v>
       </c>
-      <c r="M31" s="2" t="n">
+      <c r="Q31" s="2" t="n">
         <v>0.450140214151255</v>
       </c>
-      <c r="N31" s="2" t="n">
+      <c r="R31" s="2" t="n">
         <v>-0.108051948051948</v>
       </c>
-      <c r="O31" s="2" t="n">
+      <c r="S31" s="2" t="n">
         <v>0.281744958269162</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>4</v>
       </c>
       <c r="D32" s="2" t="n">
+        <v>492</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>583</v>
+      </c>
+      <c r="F32" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G32" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H32" s="2" t="n">
         <v>25.775</v>
       </c>
-      <c r="E32" s="2" t="n">
-        <v>3.43159341025905</v>
-      </c>
-      <c r="F32" s="2" t="n">
+      <c r="I32" s="2" t="n">
+        <v>0.825</v>
+      </c>
+      <c r="J32" s="2" t="n">
         <v>25.625</v>
       </c>
-      <c r="G32" s="2" t="n">
-        <v>3.48843326819744</v>
-      </c>
-      <c r="H32" s="2" t="n">
+      <c r="K32" s="2" t="n">
+        <v>1.27541823205828</v>
+      </c>
+      <c r="L32" s="2" t="n">
         <v>11.2</v>
-      </c>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2" t="n">
-        <v>13.9</v>
-      </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2" t="n">
-        <v>-1.26060606060606</v>
       </c>
       <c r="M32" s="2"/>
       <c r="N32" s="2" t="n">
+        <v>13.9</v>
+      </c>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2" t="n">
+        <v>-1.26060606060606</v>
+      </c>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2" t="n">
         <v>-0.921212121212121</v>
       </c>
-      <c r="O32" s="2"/>
+      <c r="S32" s="2"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D33" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E33" s="2"/>
+      <c r="D33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F33" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G33" s="2"/>
+      <c r="G33" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H33" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1833,25 +2233,37 @@
         <v>#NUM!</v>
       </c>
       <c r="O33" s="2"/>
+      <c r="P33" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S33" s="2"/>
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D34" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E34" s="2"/>
+      <c r="D34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F34" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G34" s="2"/>
+      <c r="G34" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H34" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1868,72 +2280,96 @@
         <v>#NUM!</v>
       </c>
       <c r="O34" s="2"/>
+      <c r="P34" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S34" s="2"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>10</v>
       </c>
       <c r="D35" s="2" t="n">
+        <v>866</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>978</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>14.16</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <v>14.16</v>
+      </c>
+      <c r="H35" s="2" t="n">
         <v>22.3822222222222</v>
       </c>
-      <c r="E35" s="2" t="n">
-        <v>10.0646271388683</v>
-      </c>
-      <c r="F35" s="2" t="n">
+      <c r="I35" s="2" t="n">
+        <v>3.22900526478357</v>
+      </c>
+      <c r="J35" s="2" t="n">
         <v>22.4644444444444</v>
       </c>
-      <c r="G35" s="2" t="n">
-        <v>10.2677262710776</v>
-      </c>
-      <c r="H35" s="2" t="n">
+      <c r="K35" s="2" t="n">
+        <v>4.14688571232812</v>
+      </c>
+      <c r="L35" s="2" t="n">
         <v>14.5122222222222</v>
       </c>
-      <c r="I35" s="2" t="n">
+      <c r="M35" s="2" t="n">
         <v>7.76139288043354</v>
       </c>
-      <c r="J35" s="2" t="n">
+      <c r="N35" s="2" t="n">
         <v>17.0688888888889</v>
       </c>
-      <c r="K35" s="2" t="n">
+      <c r="O35" s="2" t="n">
         <v>8.17483554030973</v>
       </c>
-      <c r="L35" s="2" t="n">
+      <c r="P35" s="2" t="n">
         <v>-0.895854408619479</v>
       </c>
-      <c r="M35" s="2" t="n">
+      <c r="Q35" s="2" t="n">
         <v>0.563701596552756</v>
       </c>
-      <c r="N35" s="2" t="n">
+      <c r="R35" s="2" t="n">
         <v>-0.512728027527365</v>
       </c>
-      <c r="O35" s="2" t="n">
+      <c r="S35" s="2" t="n">
         <v>0.280797119470041</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D36" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E36" s="2"/>
+      <c r="D36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F36" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G36" s="2"/>
+      <c r="G36" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H36" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -1950,60 +2386,84 @@
         <v>#NUM!</v>
       </c>
       <c r="O36" s="2"/>
+      <c r="P36" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S36" s="2"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D37" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>4.349</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <v>4.349</v>
+      </c>
+      <c r="H37" s="2" t="n">
         <v>11.3</v>
-      </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2" t="n">
-        <v>9</v>
-      </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2" t="n">
-        <v>7.6</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2" t="n">
-        <v>7.5</v>
+        <v>9</v>
       </c>
       <c r="K37" s="2"/>
       <c r="L37" s="2" t="n">
-        <v>-0.902439024390244</v>
+        <v>7.6</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2" t="n">
+        <v>-0.902439024390244</v>
+      </c>
+      <c r="Q37" s="2"/>
+      <c r="R37" s="2" t="n">
         <v>-0.319148936170213</v>
       </c>
-      <c r="O37" s="2"/>
+      <c r="S37" s="2"/>
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D38" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E38" s="2"/>
+      <c r="D38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F38" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G38" s="2"/>
+      <c r="G38" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H38" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2020,60 +2480,84 @@
         <v>#NUM!</v>
       </c>
       <c r="O38" s="2"/>
+      <c r="P38" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q38" s="2"/>
+      <c r="R38" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S38" s="2"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D39" s="2" t="n">
+        <v>18</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>4.349</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <v>4.349</v>
+      </c>
+      <c r="H39" s="2" t="n">
         <v>42.8</v>
-      </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2" t="n">
-        <v>39.8</v>
-      </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2" t="n">
-        <v>30.1</v>
       </c>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="n">
-        <v>33.7</v>
+        <v>39.8</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2" t="n">
-        <v>-1.48538011695906</v>
+        <v>30.1</v>
       </c>
       <c r="M39" s="2"/>
       <c r="N39" s="2" t="n">
+        <v>33.7</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2" t="n">
+        <v>-1.48538011695906</v>
+      </c>
+      <c r="Q39" s="2"/>
+      <c r="R39" s="2" t="n">
         <v>-0.583732057416267</v>
       </c>
-      <c r="O39" s="2"/>
+      <c r="S39" s="2"/>
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D40" s="2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="E40" s="2"/>
+      <c r="D40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="F40" s="2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="G40" s="2"/>
+      <c r="G40" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
       <c r="H40" s="2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2090,133 +2574,177 @@
         <v>#NUM!</v>
       </c>
       <c r="O40" s="2"/>
+      <c r="P40" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="Q40" s="2"/>
+      <c r="R40" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="S40" s="2"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>2</v>
       </c>
       <c r="D41" s="2" t="n">
+        <v>62</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>16.37</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <v>16.37</v>
+      </c>
+      <c r="H41" s="2" t="n">
         <v>12.22</v>
       </c>
-      <c r="E41" s="2" t="n">
-        <v>4.21435641587182</v>
-      </c>
-      <c r="F41" s="2" t="n">
+      <c r="I41" s="2" t="n">
+        <v>0.127279220613578</v>
+      </c>
+      <c r="J41" s="2" t="n">
         <v>13.41</v>
       </c>
-      <c r="G41" s="2" t="n">
-        <v>2.10717820793591</v>
-      </c>
-      <c r="H41" s="2" t="n">
+      <c r="K41" s="2" t="n">
+        <v>1.32228968081884</v>
+      </c>
+      <c r="L41" s="2" t="n">
         <v>7.77</v>
       </c>
-      <c r="I41" s="2" t="n">
+      <c r="M41" s="2" t="n">
         <v>2.72943217538007</v>
       </c>
-      <c r="J41" s="2" t="n">
+      <c r="N41" s="2" t="n">
         <v>10.62</v>
       </c>
-      <c r="K41" s="2" t="n">
+      <c r="O41" s="2" t="n">
         <v>0.254558441227158</v>
       </c>
-      <c r="L41" s="2" t="n">
+      <c r="P41" s="2" t="n">
         <v>-1.12098427887902</v>
       </c>
-      <c r="M41" s="2" t="n">
+      <c r="Q41" s="2" t="n">
         <v>0.434993918706694</v>
       </c>
-      <c r="N41" s="2" t="n">
+      <c r="R41" s="2" t="n">
         <v>-0.62504752851711</v>
       </c>
-      <c r="O41" s="2" t="n">
+      <c r="S41" s="2" t="n">
         <v>0.565618209475741</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>1</v>
       </c>
       <c r="D42" s="2" t="n">
+        <v>112</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>109</v>
+      </c>
+      <c r="F42" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="G42" s="2" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="H42" s="2" t="n">
         <v>76.96</v>
-      </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2" t="n">
-        <v>81.26</v>
-      </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2" t="n">
-        <v>60.58</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2" t="n">
-        <v>66.68</v>
+        <v>81.26</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2" t="n">
-        <v>-1.4469964664311</v>
+        <v>60.58</v>
       </c>
       <c r="M42" s="2"/>
       <c r="N42" s="2" t="n">
+        <v>66.68</v>
+      </c>
+      <c r="O42" s="2"/>
+      <c r="P42" s="2" t="n">
+        <v>-1.4469964664311</v>
+      </c>
+      <c r="Q42" s="2"/>
+      <c r="R42" s="2" t="n">
         <v>-1.4134755210858</v>
       </c>
-      <c r="O42" s="2"/>
+      <c r="S42" s="2"/>
     </row>
     <row r="43">
       <c r="A43" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C43" s="3" t="n">
         <v>7</v>
       </c>
       <c r="D43" s="3" t="n">
+        <v>199</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <v>196</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <v>14.0285714285714</v>
+      </c>
+      <c r="G43" s="3" t="n">
+        <v>14.0285714285714</v>
+      </c>
+      <c r="H43" s="3" t="n">
         <v>84.28</v>
       </c>
-      <c r="E43" s="3" t="n">
-        <v>3.37123122909124</v>
-      </c>
-      <c r="F43" s="3" t="n">
+      <c r="I43" s="3" t="n">
+        <v>1.03538237703115</v>
+      </c>
+      <c r="J43" s="3" t="n">
         <v>82.7183333333333</v>
       </c>
-      <c r="G43" s="3" t="n">
-        <v>2.37147563062888</v>
-      </c>
-      <c r="H43" s="3" t="n">
+      <c r="K43" s="3" t="n">
+        <v>2.8028033585442</v>
+      </c>
+      <c r="L43" s="3" t="n">
         <v>61.74</v>
       </c>
-      <c r="I43" s="3" t="n">
+      <c r="M43" s="3" t="n">
         <v>6.73220320548927</v>
       </c>
-      <c r="J43" s="3" t="n">
+      <c r="N43" s="3" t="n">
         <v>72.6</v>
       </c>
-      <c r="K43" s="3" t="n">
+      <c r="O43" s="3" t="n">
         <v>8.76907292705449</v>
       </c>
-      <c r="L43" s="3" t="n">
+      <c r="P43" s="3" t="n">
         <v>-2.17171639105173</v>
       </c>
-      <c r="M43" s="3" t="n">
+      <c r="Q43" s="3" t="n">
         <v>0.758232949400711</v>
       </c>
-      <c r="N43" s="3" t="n">
+      <c r="R43" s="3" t="n">
         <v>-0.976005277885888</v>
       </c>
-      <c r="O43" s="3" t="n">
+      <c r="S43" s="3" t="n">
         <v>0.805622084947634</v>
       </c>
     </row>

</xml_diff>